<commit_message>
feat: zamiana DbContext na elementy z repo
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbist\OneDrive\Dokumenty\GitHub\Projekt-Przychodnia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC235D8C-3F52-45A6-A486-5FEC96D93EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -161,7 +167,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -222,14 +228,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,7 +434,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
@@ -437,7 +443,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
@@ -718,35 +724,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="7" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="10" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="13" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.5">
+    <row r="1" spans="1:16" ht="61.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.25">
+    <row r="2" spans="1:16" ht="23.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -754,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.5">
+    <row r="3" spans="1:16" ht="61.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -773,65 +779,65 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="P3">
         <f>SUM(P8:P1001)</f>
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24.95" customHeight="1">
+    <row r="4" spans="1:16" ht="24.9" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.91555555555555557</v>
+        <v>0.9196428571428571</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.68</v>
+        <v>0.6830357142857143</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.79555555555555557</v>
+        <v>0.7991071428571429</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.471111111111111</v>
+        <v>1.4553571428571428</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1377777777777778</v>
+        <v>1.1428571428571428</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" t="s">
@@ -984,7 +990,7 @@
       <c r="D9">
         <v>100</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>45769</v>
       </c>
       <c r="F9" t="s">
@@ -1056,7 +1062,7 @@
         <v>27</v>
       </c>
       <c r="M10">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="N10" s="3">
         <v>45756</v>
@@ -1103,7 +1109,7 @@
         <v>28</v>
       </c>
       <c r="M11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N11" s="3">
         <v>45756</v>

</xml_diff>

<commit_message>
Validacja Emailu i Peselu
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbist\OneDrive\Dokumenty\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubac\Documents\GitHub\AI\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC235D8C-3F52-45A6-A486-5FEC96D93EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B78A88-5A8A-4C10-BF49-7E34A0BBDFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>OsobaRepository.cs</t>
+  </si>
+  <si>
+    <t>PacjentServiceImpl.cs</t>
+  </si>
+  <si>
+    <t>IPacjentService.cs</t>
   </si>
 </sst>
 </file>
@@ -727,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -775,7 +781,7 @@
       </c>
       <c r="J3">
         <f>SUM(J7:J1001)</f>
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
@@ -793,23 +799,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.9196428571428571</v>
+        <v>0.94063926940639264</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.6830357142857143</v>
+        <v>0.69863013698630139</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.7991071428571429</v>
+        <v>0.70319634703196343</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4553571428571428</v>
+        <v>1.4885844748858448</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1428571428571428</v>
+        <v>1.1689497716894977</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1100,7 +1106,7 @@
         <v>34</v>
       </c>
       <c r="J11">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K11" s="3">
         <v>45765</v>
@@ -1138,7 +1144,7 @@
         <v>35</v>
       </c>
       <c r="J12">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="K12" s="3">
         <v>45765</v>
@@ -1176,7 +1182,7 @@
         <v>36</v>
       </c>
       <c r="J13">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K13" s="3">
         <v>45765</v>
@@ -1198,6 +1204,15 @@
       </c>
     </row>
     <row r="14" spans="1:16">
+      <c r="H14" s="3">
+        <v>45770</v>
+      </c>
+      <c r="I14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
       <c r="K14" s="3">
         <v>45765</v>
       </c>
@@ -1218,6 +1233,15 @@
       </c>
     </row>
     <row r="15" spans="1:16">
+      <c r="H15" s="3">
+        <v>45770</v>
+      </c>
+      <c r="I15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
       <c r="K15" s="3">
         <v>45765</v>
       </c>
@@ -1238,6 +1262,15 @@
       </c>
     </row>
     <row r="16" spans="1:16">
+      <c r="H16" s="3">
+        <v>45770</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
       <c r="N16" s="3">
         <v>45756</v>
       </c>

</xml_diff>

<commit_message>
Zmiana Serwisów i Stworzenie Pustych testów jednostkowych
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubac\Documents\GitHub\AI\Projekt-Przychodnia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9509DFF1-9778-4DFC-81F6-71826B81E86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="0" windowWidth="11715" windowHeight="11760"/>
+    <workbookView xWindow="28680" yWindow="-8280" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -215,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -479,7 +485,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
@@ -488,7 +494,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
@@ -769,35 +775,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="7" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="10" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
+    <col min="13" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.5">
+    <row r="1" spans="1:16" ht="61.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.25">
+    <row r="2" spans="1:16" ht="23.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -805,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.5">
+    <row r="3" spans="1:16" ht="61.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -820,7 +826,7 @@
       </c>
       <c r="J3">
         <f>SUM(J7:J1001)</f>
-        <v>260</v>
+        <v>353</v>
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
@@ -831,30 +837,30 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24.95" customHeight="1">
+    <row r="4" spans="1:16" ht="24.9" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.81774081774081775</v>
+        <v>0.76822916666666663</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4067914067914067</v>
+        <v>1.3216145833333333</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.90090090090090091</v>
+        <v>1.1490885416666667</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.91822591822591826</v>
+        <v>0.86263020833333337</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.95634095634095639</v>
+        <v>0.8984375</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1632,10 +1638,72 @@
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="2:16">
+      <c r="H28" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I28" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="2:16">
+      <c r="H29" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I29" t="s">
+        <v>31</v>
+      </c>
+      <c r="J29">
+        <v>35</v>
+      </c>
       <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="H30" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="H31" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I31" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="H32" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I32" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="8:10">
+      <c r="H33" s="3">
+        <v>45788</v>
+      </c>
+      <c r="I33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
feat: add badanie, lekarz, osoba controllers
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubac\Documents\GitHub\AI\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C268B2E-E07C-4FC5-A424-5875D0EEA96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA5B91-01AB-4CAC-AC59-1FA50B7E8DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>ILekarzService.cs</t>
+  </si>
+  <si>
+    <t>program.cs</t>
+  </si>
+  <si>
+    <t>appsettings.json</t>
+  </si>
+  <si>
+    <t>BadanieController.cs</t>
+  </si>
+  <si>
+    <t>LekarzController.cs</t>
   </si>
 </sst>
 </file>
@@ -875,31 +887,31 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
-    <col min="7" max="8" width="12.5546875" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="14" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.2">
+    <row r="1" spans="1:16" ht="61.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.4">
+    <row r="2" spans="1:16" ht="23.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -907,7 +919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.2">
+    <row r="3" spans="1:16" ht="61.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -930,33 +942,33 @@
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
-        <v>276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="24.9" customHeight="1">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="24.95" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.74397339983374899</v>
+        <v>0.69622714896927262</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4484621778886118</v>
+        <v>1.3555036950602879</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.6832917705735662</v>
+        <v>1.5752625437572929</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.55070656691604325</v>
+        <v>0.51536367172306496</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.57356608478802995</v>
+        <v>0.85764294049008172</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1578,7 +1590,15 @@
       <c r="J18">
         <v>2</v>
       </c>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O18" t="s">
+        <v>93</v>
+      </c>
+      <c r="P18">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="2:16">
       <c r="B19" s="3">
@@ -1608,7 +1628,15 @@
       <c r="J19">
         <v>5</v>
       </c>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O19" t="s">
+        <v>94</v>
+      </c>
+      <c r="P19">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="2:16">
       <c r="B20" s="3">
@@ -1638,7 +1666,15 @@
       <c r="J20">
         <v>2</v>
       </c>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O20" t="s">
+        <v>95</v>
+      </c>
+      <c r="P20">
+        <v>43</v>
+      </c>
     </row>
     <row r="21" spans="2:16">
       <c r="B21" s="3">
@@ -1668,7 +1704,15 @@
       <c r="J21">
         <v>2</v>
       </c>
-      <c r="N21" s="3"/>
+      <c r="N21" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O21" t="s">
+        <v>96</v>
+      </c>
+      <c r="P21">
+        <v>37</v>
+      </c>
     </row>
     <row r="22" spans="2:16">
       <c r="B22" s="3">
@@ -1698,7 +1742,15 @@
       <c r="J22">
         <v>1</v>
       </c>
-      <c r="N22" s="3"/>
+      <c r="N22" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P22">
+        <v>62</v>
+      </c>
     </row>
     <row r="23" spans="2:16">
       <c r="B23" s="3">

</xml_diff>

<commit_message>
feat: add pacjent, recepcjonistka, wizyta, wykonane badania controllers
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,35 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA5B91-01AB-4CAC-AC59-1FA50B7E8DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAB97D5-39BF-4474-AF77-D8085EA65BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -324,6 +311,12 @@
   </si>
   <si>
     <t>LekarzController.cs</t>
+  </si>
+  <si>
+    <t>PacjentController.cs</t>
+  </si>
+  <si>
+    <t>RecepcjonistkaController.cs</t>
   </si>
 </sst>
 </file>
@@ -887,7 +880,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -938,7 +931,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>265</v>
+        <v>417</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -952,23 +945,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.69622714896927262</v>
+        <v>0.65736320235034884</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3555036950602879</v>
+        <v>1.279838413514506</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.5752625437572929</v>
+        <v>1.4873301505692251</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.51536367172306496</v>
+        <v>0.76569959603378623</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.85764294049008172</v>
+        <v>0.80976863753213368</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1590,6 +1583,15 @@
       <c r="J18">
         <v>2</v>
       </c>
+      <c r="K18" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18">
+        <v>35</v>
+      </c>
       <c r="N18" s="3">
         <v>45793</v>
       </c>
@@ -1628,6 +1630,15 @@
       <c r="J19">
         <v>5</v>
       </c>
+      <c r="K19" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L19" t="s">
+        <v>97</v>
+      </c>
+      <c r="M19">
+        <v>43</v>
+      </c>
       <c r="N19" s="3">
         <v>45793</v>
       </c>
@@ -1666,6 +1677,15 @@
       <c r="J20">
         <v>2</v>
       </c>
+      <c r="K20" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L20" t="s">
+        <v>98</v>
+      </c>
+      <c r="M20">
+        <v>35</v>
+      </c>
       <c r="N20" s="3">
         <v>45793</v>
       </c>
@@ -1703,6 +1723,15 @@
       </c>
       <c r="J21">
         <v>2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21">
+        <v>39</v>
       </c>
       <c r="N21" s="3">
         <v>45793</v>

</xml_diff>

<commit_message>
feat: tests for controllers wizyta, wykonane badania, pacjent, recepcjonistka
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FAB97D5-39BF-4474-AF77-D8085EA65BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A82EF79-50E5-4133-B60B-644F79EEA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -317,6 +317,18 @@
   </si>
   <si>
     <t>RecepcjonistkaController.cs</t>
+  </si>
+  <si>
+    <t>WykonaneBadaniaControllerTests.cs</t>
+  </si>
+  <si>
+    <t>PacjentControllerTests.cs</t>
+  </si>
+  <si>
+    <t>RecepcjonistkaControllerTests.cs</t>
+  </si>
+  <si>
+    <t>WizytaControllerTests.cs</t>
   </si>
 </sst>
 </file>
@@ -880,7 +892,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -931,7 +943,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>417</v>
+        <v>607</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -945,23 +957,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.65736320235034884</v>
+        <v>0.61448678338482665</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.279838413514506</v>
+        <v>1.1963611397185032</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4873301505692251</v>
+        <v>1.3903192584963955</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.76569959603378623</v>
+        <v>1.0418812221077927</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.80976863753213368</v>
+        <v>0.75695159629248199</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1771,6 +1783,15 @@
       <c r="J22">
         <v>1</v>
       </c>
+      <c r="K22" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L22" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22">
+        <v>44</v>
+      </c>
       <c r="N22" s="3">
         <v>45793</v>
       </c>
@@ -1809,6 +1830,15 @@
       <c r="J23">
         <v>1</v>
       </c>
+      <c r="K23" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23">
+        <v>41</v>
+      </c>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="2:16">
@@ -1839,6 +1869,15 @@
       <c r="J24">
         <v>18</v>
       </c>
+      <c r="K24" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24">
+        <v>45</v>
+      </c>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:16">
@@ -1859,6 +1898,15 @@
       </c>
       <c r="J25">
         <v>13</v>
+      </c>
+      <c r="K25" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25">
+        <v>60</v>
       </c>
       <c r="N25" s="3"/>
     </row>

</xml_diff>

<commit_message>
feat: add tests for badanie controller
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A82EF79-50E5-4133-B60B-644F79EEA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5EF6CA-26A0-41A2-99C8-E22301BAC175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>WizytaControllerTests.cs</t>
+  </si>
+  <si>
+    <t>BadanieControllerTests.cs</t>
   </si>
 </sst>
 </file>
@@ -943,7 +946,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>607</v>
+        <v>662</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -957,23 +960,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.61448678338482665</v>
+        <v>0.60309973045822107</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1963611397185032</v>
+        <v>1.1741913746630728</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3903192584963955</v>
+        <v>1.3645552560646901</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0418812221077927</v>
+        <v>1.1152291105121295</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.75695159629248199</v>
+        <v>0.74292452830188682</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1928,6 +1931,15 @@
       </c>
       <c r="J26">
         <v>41</v>
+      </c>
+      <c r="K26" s="3">
+        <v>45793</v>
+      </c>
+      <c r="L26" t="s">
+        <v>103</v>
+      </c>
+      <c r="M26">
+        <v>55</v>
       </c>
       <c r="N26" s="3"/>
     </row>

</xml_diff>

<commit_message>
test: lekarz, osoba Controllers tests
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5EF6CA-26A0-41A2-99C8-E22301BAC175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8A6E4F-F6A7-4C5D-9D4A-8288B7D911D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -332,6 +345,12 @@
   </si>
   <si>
     <t>BadanieControllerTests.cs</t>
+  </si>
+  <si>
+    <t>LekarzControllerTest.cs</t>
+  </si>
+  <si>
+    <t>OsobaControllerTest.cs</t>
   </si>
 </sst>
 </file>
@@ -895,7 +914,7 @@
   <dimension ref="A1:P50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -950,7 +969,7 @@
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
-        <v>441</v>
+        <v>657</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="24.95" customHeight="1">
@@ -960,23 +979,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.60309973045822107</v>
+        <v>0.56218592964824121</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1741913746630728</v>
+        <v>1.0945351758793971</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3645552560646901</v>
+        <v>1.2719849246231156</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1152291105121295</v>
+        <v>1.039572864321608</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.74292452830188682</v>
+        <v>1.0317211055276383</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1842,7 +1861,15 @@
       <c r="M23">
         <v>41</v>
       </c>
-      <c r="N23" s="3"/>
+      <c r="N23" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O23" t="s">
+        <v>104</v>
+      </c>
+      <c r="P23">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="2:16">
       <c r="B24" s="3">
@@ -1881,7 +1908,15 @@
       <c r="M24">
         <v>45</v>
       </c>
-      <c r="N24" s="3"/>
+      <c r="N24" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O24" t="s">
+        <v>105</v>
+      </c>
+      <c r="P24">
+        <v>126</v>
+      </c>
     </row>
     <row r="25" spans="2:16">
       <c r="B25" s="3">

</xml_diff>

<commit_message>
naprawa błędów i hostowanie na serwerze
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8A6E4F-F6A7-4C5D-9D4A-8288B7D911D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E365F34-73FD-4B5D-A256-A64F813D9F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="107">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>OsobaControllerTest.cs</t>
+  </si>
+  <si>
+    <t>host aplikacji na serwerze</t>
   </si>
 </sst>
 </file>
@@ -913,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -953,7 +956,7 @@
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>358</v>
+        <v>658</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -979,23 +982,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.56218592964824121</v>
+        <v>0.94431687715269808</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0945351758793971</v>
+        <v>1.0002870264064294</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2719849246231156</v>
+        <v>1.1624569460390355</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.039572864321608</v>
+        <v>0.9500574052812859</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0317211055276383</v>
+        <v>0.94288174512055112</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2183,7 +2186,13 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="3">
-        <v>45790</v>
+        <v>45798</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37">
+        <v>300</v>
       </c>
       <c r="H37" s="3">
         <v>45790</v>
@@ -2196,9 +2205,7 @@
       </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="3">
-        <v>45790</v>
-      </c>
+      <c r="B38" s="3"/>
       <c r="H38" s="3">
         <v>45790</v>
       </c>

</xml_diff>

<commit_message>
feat: add login and register
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubac\Documents\GitHub\AI\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35EED1A-7B96-46DD-8938-2B44C6EE9E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6989D184-16D4-4CFF-9732-24A4331ECA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -369,13 +369,37 @@
   </si>
   <si>
     <t>Raport</t>
+  </si>
+  <si>
+    <t>poprawki/deklaracje</t>
+  </si>
+  <si>
+    <t>LoginDTO.cs</t>
+  </si>
+  <si>
+    <t>RegisterDTO.cs</t>
+  </si>
+  <si>
+    <t>AuthResponseDTO.cs</t>
+  </si>
+  <si>
+    <t>ChangePasswordDTO.cs</t>
+  </si>
+  <si>
+    <t>IAuthService.cs</t>
+  </si>
+  <si>
+    <t>AuthService.cs</t>
+  </si>
+  <si>
+    <t>AuthController.cs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,11 +408,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="48"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,7 +429,8 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -422,14 +456,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -440,6 +474,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,32 +968,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
-    <col min="7" max="8" width="12.5546875" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="14" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.2">
+    <row r="1" spans="1:16" ht="61.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.4">
+    <row r="2" spans="1:16" ht="23.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -964,7 +1001,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.2">
+    <row r="3" spans="1:16" ht="61.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -987,33 +1024,33 @@
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
-        <v>657</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="24.9" customHeight="1">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="24.95" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.86397058823529416</v>
+        <v>0.78389325708839652</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.9151785714285714</v>
+        <v>0.83035501548725277</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3563550420168067</v>
+        <v>1.2306409340004765</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0018382352941178</v>
+        <v>0.90898260662377894</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.86265756302521013</v>
+        <v>1.2461281868000953</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1964,7 +2001,15 @@
       <c r="M25">
         <v>60</v>
       </c>
-      <c r="N25" s="3"/>
+      <c r="N25" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="2:16">
       <c r="B26" s="3">
@@ -1994,7 +2039,15 @@
       <c r="M26">
         <v>55</v>
       </c>
-      <c r="N26" s="3"/>
+      <c r="N26" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P26">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="3">
@@ -2024,7 +2077,15 @@
       <c r="M27">
         <v>28</v>
       </c>
-      <c r="N27" s="3"/>
+      <c r="N27" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O27" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="P27">
+        <v>25</v>
+      </c>
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="3">
@@ -2054,7 +2115,15 @@
       <c r="M28">
         <v>72</v>
       </c>
-      <c r="N28" s="3"/>
+      <c r="N28" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O28" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="P28">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="3">
@@ -2075,7 +2144,15 @@
       <c r="J29">
         <v>35</v>
       </c>
-      <c r="N29" s="3"/>
+      <c r="N29" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="P29">
+        <v>9</v>
+      </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="3">
@@ -2096,6 +2173,15 @@
       <c r="J30">
         <v>20</v>
       </c>
+      <c r="N30" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O30" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="P30">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="2:16">
       <c r="B31" s="3">
@@ -2116,6 +2202,15 @@
       <c r="J31">
         <v>9</v>
       </c>
+      <c r="N31" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="P31">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="2:16">
       <c r="B32" s="3">
@@ -2136,8 +2231,17 @@
       <c r="J32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="2:10">
+      <c r="N32" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O32" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="P32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16">
       <c r="B33" s="3">
         <v>45790</v>
       </c>
@@ -2156,8 +2260,17 @@
       <c r="J33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="2:10">
+      <c r="N33" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O33" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="P33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
       <c r="B34" s="3">
         <v>45790</v>
       </c>
@@ -2176,8 +2289,17 @@
       <c r="J34">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="2:10">
+      <c r="N34" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O34" t="s">
+        <v>118</v>
+      </c>
+      <c r="P34">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="3">
         <v>45790</v>
       </c>
@@ -2196,8 +2318,17 @@
       <c r="J35">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="2:10">
+      <c r="N35" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
       <c r="B36" s="3">
         <v>45790</v>
       </c>
@@ -2216,8 +2347,17 @@
       <c r="J36">
         <v>28</v>
       </c>
-    </row>
-    <row r="37" spans="2:10">
+      <c r="N36" s="3">
+        <v>45862</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="P36">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
       <c r="B37" s="3">
         <v>45798</v>
       </c>
@@ -2237,7 +2377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:10">
+    <row r="38" spans="2:16">
       <c r="B38" s="3"/>
       <c r="H38" s="3">
         <v>45790</v>
@@ -2249,7 +2389,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:16">
       <c r="H39" s="3">
         <v>45790</v>
       </c>
@@ -2260,7 +2400,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="2:10">
+    <row r="40" spans="2:16">
       <c r="H40" s="3">
         <v>45790</v>
       </c>
@@ -2271,7 +2411,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:10">
+    <row r="41" spans="2:16">
       <c r="H41" s="3">
         <v>45790</v>
       </c>
@@ -2282,7 +2422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:16">
       <c r="H42" s="3">
         <v>45790</v>
       </c>
@@ -2293,7 +2433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="2:10">
+    <row r="43" spans="2:16">
       <c r="H43" s="3">
         <v>45790</v>
       </c>
@@ -2304,7 +2444,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="2:10">
+    <row r="44" spans="2:16">
       <c r="H44" s="3">
         <v>45790</v>
       </c>
@@ -2315,7 +2455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="2:10">
+    <row r="45" spans="2:16">
       <c r="H45" s="3">
         <v>45790</v>
       </c>
@@ -2326,7 +2466,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:10">
+    <row r="46" spans="2:16">
       <c r="H46" s="3">
         <v>45790</v>
       </c>
@@ -2337,7 +2477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:10">
+    <row r="47" spans="2:16">
       <c r="H47" s="3">
         <v>45790</v>
       </c>
@@ -2348,7 +2488,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:10">
+    <row r="48" spans="2:16">
       <c r="H48" s="3">
         <v>45790</v>
       </c>

</xml_diff>

<commit_message>
generacja recepty w formacie pdf
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6989D184-16D4-4CFF-9732-24A4331ECA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CB40C3-158A-4295-A749-8A9C4EBB88C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39210" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="126">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -393,6 +393,24 @@
   </si>
   <si>
     <t>AuthController.cs</t>
+  </si>
+  <si>
+    <t>PdfGenratorService</t>
+  </si>
+  <si>
+    <t>wykonaneBadaniaService</t>
+  </si>
+  <si>
+    <t>wykonaneBadania.cs</t>
+  </si>
+  <si>
+    <t>wykonaneBadaniaDTO</t>
+  </si>
+  <si>
+    <t>DBInit.cs</t>
+  </si>
+  <si>
+    <t>wykonaneBadaniaControler</t>
   </si>
 </sst>
 </file>
@@ -469,14 +487,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1008,7 +1026,7 @@
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>658</v>
+        <v>725</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -1034,51 +1052,51 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.78389325708839652</v>
+        <v>0.85014071294559101</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>0.83035501548725277</v>
+        <v>0.81730769230769229</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2306409340004765</v>
+        <v>1.2113039399624765</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.90898260662377894</v>
+        <v>0.89469981238273921</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2461281868000953</v>
+        <v>1.2265478424015008</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" t="s">
@@ -2004,7 +2022,7 @@
       <c r="N25" s="3">
         <v>45862</v>
       </c>
-      <c r="O25" s="6" t="s">
+      <c r="O25" s="4" t="s">
         <v>35</v>
       </c>
       <c r="P25">
@@ -2042,7 +2060,7 @@
       <c r="N26" s="3">
         <v>45862</v>
       </c>
-      <c r="O26" s="6" t="s">
+      <c r="O26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="P26">
@@ -2080,7 +2098,7 @@
       <c r="N27" s="3">
         <v>45862</v>
       </c>
-      <c r="O27" s="6" t="s">
+      <c r="O27" s="4" t="s">
         <v>112</v>
       </c>
       <c r="P27">
@@ -2118,7 +2136,7 @@
       <c r="N28" s="3">
         <v>45862</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="O28" s="4" t="s">
         <v>94</v>
       </c>
       <c r="P28">
@@ -2147,7 +2165,7 @@
       <c r="N29" s="3">
         <v>45862</v>
       </c>
-      <c r="O29" s="6" t="s">
+      <c r="O29" s="4" t="s">
         <v>113</v>
       </c>
       <c r="P29">
@@ -2176,7 +2194,7 @@
       <c r="N30" s="3">
         <v>45862</v>
       </c>
-      <c r="O30" s="6" t="s">
+      <c r="O30" s="4" t="s">
         <v>114</v>
       </c>
       <c r="P30">
@@ -2205,7 +2223,7 @@
       <c r="N31" s="3">
         <v>45862</v>
       </c>
-      <c r="O31" s="6" t="s">
+      <c r="O31" s="4" t="s">
         <v>115</v>
       </c>
       <c r="P31">
@@ -2234,7 +2252,7 @@
       <c r="N32" s="3">
         <v>45862</v>
       </c>
-      <c r="O32" s="6" t="s">
+      <c r="O32" s="4" t="s">
         <v>116</v>
       </c>
       <c r="P32">
@@ -2263,7 +2281,7 @@
       <c r="N33" s="3">
         <v>45862</v>
       </c>
-      <c r="O33" s="6" t="s">
+      <c r="O33" s="4" t="s">
         <v>117</v>
       </c>
       <c r="P33">
@@ -2321,7 +2339,7 @@
       <c r="N35" s="3">
         <v>45862</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="O35" s="4" t="s">
         <v>93</v>
       </c>
       <c r="P35">
@@ -2350,7 +2368,7 @@
       <c r="N36" s="3">
         <v>45862</v>
       </c>
-      <c r="O36" s="6" t="s">
+      <c r="O36" s="4" t="s">
         <v>119</v>
       </c>
       <c r="P36">
@@ -2378,7 +2396,15 @@
       </c>
     </row>
     <row r="38" spans="2:16">
-      <c r="B38" s="3"/>
+      <c r="B38" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C38" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38">
+        <v>28</v>
+      </c>
       <c r="H38" s="3">
         <v>45790</v>
       </c>
@@ -2390,6 +2416,15 @@
       </c>
     </row>
     <row r="39" spans="2:16">
+      <c r="B39" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39">
+        <v>25</v>
+      </c>
       <c r="H39" s="3">
         <v>45790</v>
       </c>
@@ -2401,6 +2436,15 @@
       </c>
     </row>
     <row r="40" spans="2:16">
+      <c r="B40" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
       <c r="H40" s="3">
         <v>45790</v>
       </c>
@@ -2412,6 +2456,15 @@
       </c>
     </row>
     <row r="41" spans="2:16">
+      <c r="B41" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
       <c r="H41" s="3">
         <v>45790</v>
       </c>
@@ -2423,6 +2476,15 @@
       </c>
     </row>
     <row r="42" spans="2:16">
+      <c r="B42" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
       <c r="H42" s="3">
         <v>45790</v>
       </c>
@@ -2434,6 +2496,15 @@
       </c>
     </row>
     <row r="43" spans="2:16">
+      <c r="B43" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
       <c r="H43" s="3">
         <v>45790</v>
       </c>
@@ -2445,6 +2516,15 @@
       </c>
     </row>
     <row r="44" spans="2:16">
+      <c r="B44" s="3">
+        <v>45874</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
       <c r="H44" s="3">
         <v>45790</v>
       </c>

</xml_diff>

<commit_message>
fix: harmonogram files updated, error fix
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B525A51-AA8A-4ED0-AC63-267095BB0AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="170">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -521,12 +527,15 @@
   </si>
   <si>
     <t>home.component.css</t>
+  </si>
+  <si>
+    <t>HarmonogramControllerTest.cs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -826,7 +835,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
@@ -835,7 +844,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
@@ -1116,11 +1125,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1171,7 +1180,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>778</v>
+        <v>848</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -1185,23 +1194,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.69967187801582709</v>
+        <v>0.69034469624833361</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.5431383902721483</v>
+        <v>1.5225671300704628</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.996911793090137</v>
+        <v>0.9836221672062464</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.75082030496043239</v>
+        <v>0.80746524471529235</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0094576336614554</v>
+        <v>0.99600076175966479</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2575,6 +2584,15 @@
       <c r="J34">
         <v>50</v>
       </c>
+      <c r="K34" s="3">
+        <v>45887</v>
+      </c>
+      <c r="L34" t="s">
+        <v>102</v>
+      </c>
+      <c r="M34">
+        <v>10</v>
+      </c>
       <c r="N34" s="3">
         <v>45862</v>
       </c>
@@ -2613,6 +2631,15 @@
       <c r="J35">
         <v>28</v>
       </c>
+      <c r="K35" s="3">
+        <v>45887</v>
+      </c>
+      <c r="L35" t="s">
+        <v>169</v>
+      </c>
+      <c r="M35">
+        <v>48</v>
+      </c>
       <c r="N35" s="3">
         <v>45862</v>
       </c>
@@ -2651,6 +2678,15 @@
       <c r="J36">
         <v>28</v>
       </c>
+      <c r="K36" s="3">
+        <v>45887</v>
+      </c>
+      <c r="L36" t="s">
+        <v>145</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
       <c r="N36" s="3">
         <v>45862</v>
       </c>
@@ -2689,6 +2725,15 @@
       <c r="J37">
         <v>44</v>
       </c>
+      <c r="K37" s="3">
+        <v>45887</v>
+      </c>
+      <c r="L37" t="s">
+        <v>151</v>
+      </c>
+      <c r="M37">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="3">
@@ -2718,6 +2763,15 @@
       <c r="J38">
         <v>52</v>
       </c>
+      <c r="K38" s="3">
+        <v>45887</v>
+      </c>
+      <c r="L38" t="s">
+        <v>155</v>
+      </c>
+      <c r="M38">
+        <v>4</v>
+      </c>
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="3">
@@ -2747,6 +2801,7 @@
       <c r="J39">
         <v>75</v>
       </c>
+      <c r="K39" s="3"/>
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="3">

</xml_diff>

<commit_message>
feat: add login component
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\GitHub\Projekt-Przychodnia\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8A7D34-CAC8-4576-869A-E99E9A2F8FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="185">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -557,18 +576,38 @@
   </si>
   <si>
     <t>WizytaWidokDTO.cs</t>
+  </si>
+  <si>
+    <t>login.component.ts</t>
+  </si>
+  <si>
+    <t>login.component.css</t>
+  </si>
+  <si>
+    <t>login.component.html</t>
+  </si>
+  <si>
+    <t>register.component.css</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -646,31 +685,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -678,6 +714,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -876,7 +915,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
-    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="headerRow" dxfId="15"/>
       <tableStyleElement type="totalRow" dxfId="14"/>
@@ -885,7 +924,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="11"/>
       <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10">
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
       <tableStyleElement type="firstRowStripe" dxfId="7"/>
@@ -1166,11 +1205,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1225,7 +1264,7 @@
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
-        <v>1250</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="24.95" customHeight="1">
@@ -1235,51 +1274,51 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.67985611510791366</v>
+        <v>0.65693430656934304</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.5242805755395683</v>
+        <v>1.47288842544317</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.9289568345323741</v>
+        <v>0.89763642683350708</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.7428057553956835</v>
+        <v>0.71776155717761558</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1241007194244603</v>
+        <v>1.2547792839763643</v>
       </c>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" t="s">
@@ -2755,7 +2794,7 @@
         <v>175</v>
       </c>
       <c r="P37">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="2:16">
@@ -2869,7 +2908,7 @@
         <v>130</v>
       </c>
       <c r="P40">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:16">
@@ -2941,11 +2980,11 @@
       <c r="N42" s="3">
         <v>45869</v>
       </c>
-      <c r="O42" s="9" t="s">
+      <c r="O42" t="s">
         <v>176</v>
       </c>
       <c r="P42">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="2:16">
@@ -2979,7 +3018,7 @@
       <c r="N43" s="3">
         <v>45869</v>
       </c>
-      <c r="O43" s="9" t="s">
+      <c r="O43" t="s">
         <v>177</v>
       </c>
       <c r="P43">
@@ -3084,7 +3123,15 @@
       <c r="J46">
         <v>6</v>
       </c>
-      <c r="N46" s="3"/>
+      <c r="N46" s="3">
+        <v>45896</v>
+      </c>
+      <c r="O46" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="P46">
+        <v>50</v>
+      </c>
     </row>
     <row r="47" spans="2:16">
       <c r="C47" t="s">
@@ -3111,7 +3158,15 @@
       <c r="J47">
         <v>6</v>
       </c>
-      <c r="N47" s="3"/>
+      <c r="N47" s="3">
+        <v>45896</v>
+      </c>
+      <c r="O47" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="P47">
+        <v>19</v>
+      </c>
     </row>
     <row r="48" spans="2:16">
       <c r="C48" t="s">
@@ -3138,9 +3193,17 @@
       <c r="J48">
         <v>6</v>
       </c>
-      <c r="N48" s="3"/>
-    </row>
-    <row r="49" spans="3:14">
+      <c r="N48" s="3">
+        <v>45896</v>
+      </c>
+      <c r="O48" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="P48">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="3:16">
       <c r="C49" t="s">
         <v>20</v>
       </c>
@@ -3165,9 +3228,17 @@
       <c r="J49">
         <v>6</v>
       </c>
-      <c r="N49" s="3"/>
-    </row>
-    <row r="50" spans="3:14">
+      <c r="N49" s="3">
+        <v>45896</v>
+      </c>
+      <c r="O49" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="P49">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="3:16">
       <c r="E50" s="3">
         <v>45880</v>
       </c>
@@ -3186,8 +3257,17 @@
       <c r="J50">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="3:14">
+      <c r="N50" s="3">
+        <v>45896</v>
+      </c>
+      <c r="O50" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="P50">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="3:16">
       <c r="E51" s="3">
         <v>45880</v>
       </c>
@@ -3207,7 +3287,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="3:14">
+    <row r="52" spans="3:16">
       <c r="E52" s="3">
         <v>45880</v>
       </c>
@@ -3227,7 +3307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="3:14">
+    <row r="53" spans="3:16">
       <c r="E53" s="3">
         <v>45880</v>
       </c>
@@ -3247,7 +3327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="3:14">
+    <row r="54" spans="3:16">
       <c r="E54" s="3">
         <v>45880</v>
       </c>
@@ -3258,7 +3338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:14">
+    <row r="55" spans="3:16">
       <c r="E55" s="3">
         <v>45880</v>
       </c>
@@ -3269,7 +3349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="3:14">
+    <row r="56" spans="3:16">
       <c r="E56" s="3">
         <v>45880</v>
       </c>
@@ -3280,7 +3360,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="3:14">
+    <row r="57" spans="3:16">
       <c r="E57" s="3">
         <v>45880</v>
       </c>
@@ -3291,7 +3371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="3:14">
+    <row r="58" spans="3:16">
       <c r="E58" s="3">
         <v>45880</v>
       </c>
@@ -3302,7 +3382,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="3:14">
+    <row r="59" spans="3:16">
       <c r="E59" s="3">
         <v>45880</v>
       </c>
@@ -3313,7 +3393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="3:14">
+    <row r="60" spans="3:16">
       <c r="E60" s="3">
         <v>45880</v>
       </c>
@@ -3324,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:14">
+    <row r="61" spans="3:16">
       <c r="E61" s="3">
         <v>45881</v>
       </c>
@@ -3335,7 +3415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="3:14">
+    <row r="62" spans="3:16">
       <c r="E62" s="3">
         <v>45881</v>
       </c>
@@ -3346,7 +3426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="3:14">
+    <row r="63" spans="3:16">
       <c r="E63" s="3">
         <v>45881</v>
       </c>
@@ -3357,7 +3437,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="3:14">
+    <row r="64" spans="3:16">
       <c r="E64" s="3">
         <v>45881</v>
       </c>

</xml_diff>

<commit_message>
feat: routing dla dodawania wizyt & update excela
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE58BB4B-EB26-4C07-81B2-77C9193DE281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E432A-8A62-41C9-8650-08572EB2D4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="193">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -1220,7 +1220,7 @@
   <dimension ref="A1:P112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1080</v>
+        <v>1087</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -1285,23 +1285,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.62916111850865508</v>
+        <v>0.62842892768079806</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4106191744340879</v>
+        <v>1.4089775561097257</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.85968708388814918</v>
+        <v>0.85868661679135494</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.89880159786950731</v>
+        <v>0.90357439733998335</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2017310252996005</v>
+        <v>1.2003325020781379</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -2917,7 +2917,7 @@
         <v>166</v>
       </c>
       <c r="M39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N39" s="3">
         <v>45869</v>
@@ -3448,7 +3448,7 @@
         <v>130</v>
       </c>
       <c r="M51">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="3:16">
@@ -3519,6 +3519,15 @@
       <c r="G54">
         <v>1</v>
       </c>
+      <c r="K54" s="3">
+        <v>45906</v>
+      </c>
+      <c r="L54" t="s">
+        <v>189</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
     </row>
     <row r="55" spans="3:16">
       <c r="E55" s="3">
@@ -3530,6 +3539,9 @@
       <c r="G55">
         <v>5</v>
       </c>
+      <c r="K55" s="3">
+        <v>45906</v>
+      </c>
     </row>
     <row r="56" spans="3:16">
       <c r="E56" s="3">
@@ -3541,6 +3553,7 @@
       <c r="G56">
         <v>49</v>
       </c>
+      <c r="K56" s="3"/>
     </row>
     <row r="57" spans="3:16">
       <c r="E57" s="3">

</xml_diff>

<commit_message>
panel pacjenta i jego obsługa
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E432A-8A62-41C9-8650-08572EB2D4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB5E122-EF35-464D-ACD3-7DB6FF75D625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39210" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="209">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -599,6 +612,54 @@
   </si>
   <si>
     <t>recepcja-home.component.css</t>
+  </si>
+  <si>
+    <t>pacjent.model.ts</t>
+  </si>
+  <si>
+    <t>WykonaneBadanie.cs</t>
+  </si>
+  <si>
+    <t>WykonaneBadanieRepository.cs</t>
+  </si>
+  <si>
+    <t>IWykonaneBadanieRepository.cs</t>
+  </si>
+  <si>
+    <t>IWykonaneBadanieService.cs</t>
+  </si>
+  <si>
+    <t>WykonaneBadanieService.cs</t>
+  </si>
+  <si>
+    <t>WykonaneBadanieController.cs</t>
+  </si>
+  <si>
+    <t>WykonaneBadanieDTO.cs</t>
+  </si>
+  <si>
+    <t>wykonane-badania.model.ts</t>
+  </si>
+  <si>
+    <t>pacjent.service.ts</t>
+  </si>
+  <si>
+    <t>wykonane-badania.service.ts</t>
+  </si>
+  <si>
+    <t>pacjent-home</t>
+  </si>
+  <si>
+    <t>pacjent-dane</t>
+  </si>
+  <si>
+    <t>pacjent-shell</t>
+  </si>
+  <si>
+    <t>pacjent-wizyty</t>
+  </si>
+  <si>
+    <t>pacjent-badania</t>
   </si>
 </sst>
 </file>
@@ -1219,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M61" sqref="M61"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1259,7 +1320,7 @@
       <c r="B3" s="1"/>
       <c r="D3">
         <f>SUM(D7:D1001)</f>
-        <v>756</v>
+        <v>1008</v>
       </c>
       <c r="G3">
         <f>SUM(G7:G1001)</f>
@@ -1285,23 +1346,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.62842892768079806</v>
+        <v>0.80421254188606994</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.4089775561097257</v>
+        <v>1.3523216850167545</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.85868661679135494</v>
+        <v>0.82415828945268865</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.90357439733998335</v>
+        <v>0.86724110419658529</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2003325020781379</v>
+        <v>1.1520663794479018</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3165,6 +3226,9 @@
       </c>
     </row>
     <row r="45" spans="2:16">
+      <c r="B45" s="3">
+        <v>45887</v>
+      </c>
       <c r="C45" t="s">
         <v>155</v>
       </c>
@@ -3209,6 +3273,9 @@
       </c>
     </row>
     <row r="46" spans="2:16">
+      <c r="B46" s="3">
+        <v>45887</v>
+      </c>
       <c r="C46" t="s">
         <v>99</v>
       </c>
@@ -3253,6 +3320,9 @@
       </c>
     </row>
     <row r="47" spans="2:16">
+      <c r="B47" s="3">
+        <v>45887</v>
+      </c>
       <c r="C47" t="s">
         <v>150</v>
       </c>
@@ -3297,6 +3367,9 @@
       </c>
     </row>
     <row r="48" spans="2:16">
+      <c r="B48" s="3">
+        <v>45887</v>
+      </c>
       <c r="C48" t="s">
         <v>15</v>
       </c>
@@ -3340,7 +3413,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="3:16">
+    <row r="49" spans="2:16">
+      <c r="B49" s="3">
+        <v>45887</v>
+      </c>
       <c r="C49" t="s">
         <v>20</v>
       </c>
@@ -3384,7 +3460,16 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="3:16">
+    <row r="50" spans="2:16">
+      <c r="B50" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
       <c r="E50" s="3">
         <v>45880</v>
       </c>
@@ -3422,7 +3507,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="3:16">
+    <row r="51" spans="2:16">
+      <c r="B51" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
       <c r="E51" s="3">
         <v>45880</v>
       </c>
@@ -3451,7 +3545,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="3:16">
+    <row r="52" spans="2:16">
+      <c r="B52" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C52" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
       <c r="E52" s="3">
         <v>45880</v>
       </c>
@@ -3480,7 +3583,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:16">
+    <row r="53" spans="2:16">
+      <c r="B53" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C53" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
       <c r="E53" s="3">
         <v>45880</v>
       </c>
@@ -3509,7 +3621,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="3:16">
+    <row r="54" spans="2:16">
+      <c r="B54" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54">
+        <v>4</v>
+      </c>
       <c r="E54" s="3">
         <v>45880</v>
       </c>
@@ -3529,7 +3650,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="3:16">
+    <row r="55" spans="2:16">
+      <c r="B55" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
       <c r="E55" s="3">
         <v>45880</v>
       </c>
@@ -3543,7 +3673,16 @@
         <v>45906</v>
       </c>
     </row>
-    <row r="56" spans="3:16">
+    <row r="56" spans="2:16">
+      <c r="B56" s="3">
+        <v>45905</v>
+      </c>
+      <c r="C56" t="s">
+        <v>193</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
       <c r="E56" s="3">
         <v>45880</v>
       </c>
@@ -3555,7 +3694,16 @@
       </c>
       <c r="K56" s="3"/>
     </row>
-    <row r="57" spans="3:16">
+    <row r="57" spans="2:16">
+      <c r="B57" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
       <c r="E57" s="3">
         <v>45880</v>
       </c>
@@ -3566,7 +3714,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="3:16">
+    <row r="58" spans="2:16">
+      <c r="B58" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C58" t="s">
+        <v>195</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
       <c r="E58" s="3">
         <v>45880</v>
       </c>
@@ -3577,7 +3734,16 @@
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="3:16">
+    <row r="59" spans="2:16">
+      <c r="B59" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C59" t="s">
+        <v>196</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
       <c r="E59" s="3">
         <v>45880</v>
       </c>
@@ -3588,7 +3754,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="3:16">
+    <row r="60" spans="2:16">
+      <c r="B60" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C60" t="s">
+        <v>197</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
       <c r="E60" s="3">
         <v>45880</v>
       </c>
@@ -3599,7 +3774,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:16">
+    <row r="61" spans="2:16">
+      <c r="B61" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C61" t="s">
+        <v>198</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
       <c r="E61" s="3">
         <v>45881</v>
       </c>
@@ -3610,7 +3794,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="3:16">
+    <row r="62" spans="2:16">
+      <c r="B62" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C62" t="s">
+        <v>199</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
       <c r="E62" s="3">
         <v>45881</v>
       </c>
@@ -3621,7 +3814,16 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="3:16">
+    <row r="63" spans="2:16">
+      <c r="B63" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
       <c r="E63" s="3">
         <v>45881</v>
       </c>
@@ -3632,7 +3834,16 @@
         <v>43</v>
       </c>
     </row>
-    <row r="64" spans="3:16">
+    <row r="64" spans="2:16">
+      <c r="B64" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C64" t="s">
+        <v>124</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
       <c r="E64" s="3">
         <v>45881</v>
       </c>
@@ -3643,7 +3854,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="5:7">
+    <row r="65" spans="2:7">
+      <c r="B65" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C65" t="s">
+        <v>200</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
       <c r="E65" s="3">
         <v>45881</v>
       </c>
@@ -3654,7 +3874,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="5:7">
+    <row r="66" spans="2:7">
+      <c r="B66" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C66" t="s">
+        <v>201</v>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
       <c r="E66" s="3">
         <v>45881</v>
       </c>
@@ -3665,7 +3894,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="5:7">
+    <row r="67" spans="2:7">
+      <c r="B67" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D67">
+        <v>13</v>
+      </c>
       <c r="E67" s="3">
         <v>45882</v>
       </c>
@@ -3676,7 +3914,16 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="5:7">
+    <row r="68" spans="2:7">
+      <c r="B68" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C68" t="s">
+        <v>203</v>
+      </c>
+      <c r="D68">
+        <v>29</v>
+      </c>
       <c r="E68" s="3">
         <v>45882</v>
       </c>
@@ -3687,7 +3934,16 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="5:7">
+    <row r="69" spans="2:7">
+      <c r="B69" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C69" t="s">
+        <v>130</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
       <c r="E69" s="3">
         <v>45882</v>
       </c>
@@ -3698,7 +3954,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="5:7">
+    <row r="70" spans="2:7">
+      <c r="B70" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
       <c r="E70" s="3">
         <v>45882</v>
       </c>
@@ -3709,7 +3974,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="5:7">
+    <row r="71" spans="2:7">
+      <c r="B71" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C71" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71">
+        <v>15</v>
+      </c>
       <c r="E71" s="3">
         <v>45882</v>
       </c>
@@ -3720,7 +3994,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="5:7">
+    <row r="72" spans="2:7">
+      <c r="B72" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C72" t="s">
+        <v>206</v>
+      </c>
+      <c r="D72">
+        <v>62</v>
+      </c>
       <c r="E72" s="3">
         <v>45882</v>
       </c>
@@ -3731,7 +4014,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="5:7">
+    <row r="73" spans="2:7">
+      <c r="B73" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C73" t="s">
+        <v>207</v>
+      </c>
+      <c r="D73">
+        <v>38</v>
+      </c>
       <c r="E73" s="3">
         <v>45882</v>
       </c>
@@ -3742,7 +4034,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="5:7">
+    <row r="74" spans="2:7">
+      <c r="B74" s="3">
+        <v>45906</v>
+      </c>
+      <c r="C74" t="s">
+        <v>208</v>
+      </c>
+      <c r="D74">
+        <v>31</v>
+      </c>
       <c r="E74" s="3">
         <v>45882</v>
       </c>
@@ -3753,7 +4054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="5:7">
+    <row r="75" spans="2:7">
       <c r="E75" s="3">
         <v>45882</v>
       </c>
@@ -3764,7 +4065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="5:7">
+    <row r="76" spans="2:7">
       <c r="E76" s="3">
         <v>45883</v>
       </c>
@@ -3775,7 +4076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="5:7">
+    <row r="77" spans="2:7">
       <c r="E77" s="3">
         <v>45883</v>
       </c>
@@ -3786,7 +4087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="5:7">
+    <row r="78" spans="2:7">
       <c r="E78" s="3">
         <v>45883</v>
       </c>
@@ -3797,7 +4098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="5:7">
+    <row r="79" spans="2:7">
       <c r="E79" s="3">
         <v>45883</v>
       </c>
@@ -3808,7 +4109,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="5:7">
+    <row r="80" spans="2:7">
       <c r="E80" s="3">
         <v>45883</v>
       </c>

</xml_diff>

<commit_message>
feat: poprawka strony glownej
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,35 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB5E122-EF35-464D-ACD3-7DB6FF75D625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278A739F-F855-4456-8D64-3167D54A67E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39210" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="209">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -1280,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -1332,7 +1319,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1087</v>
+        <v>1153</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -1346,23 +1333,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.80421254188606994</v>
+        <v>0.7958313595452392</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.3523216850167545</v>
+        <v>1.3382283278067266</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.82415828945268865</v>
+        <v>0.81556924048634138</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.86724110419658529</v>
+        <v>0.91031106900363179</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1520663794479018</v>
+        <v>1.140060003158061</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3670,7 +3657,13 @@
         <v>5</v>
       </c>
       <c r="K55" s="3">
-        <v>45906</v>
+        <v>45907</v>
+      </c>
+      <c r="L55" t="s">
+        <v>176</v>
+      </c>
+      <c r="M55">
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="2:16">
@@ -3692,7 +3685,15 @@
       <c r="G56">
         <v>49</v>
       </c>
-      <c r="K56" s="3"/>
+      <c r="K56" s="3">
+        <v>45907</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M56">
+        <v>47</v>
+      </c>
     </row>
     <row r="57" spans="2:16">
       <c r="B57" s="3">

</xml_diff>

<commit_message>
feat: poprawa PDM & update excela
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,35 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubac\Documents\GitHub\AI\przych\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Documents\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AEBA37-20A2-4D25-9F40-9EFFD71014C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBD6152-31F4-4AA4-85A7-379271AA0B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="214">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -669,6 +656,12 @@
   </si>
   <si>
     <t>diagramy</t>
+  </si>
+  <si>
+    <t>sprawozdanie</t>
+  </si>
+  <si>
+    <t>diagram PDM poprawa</t>
   </si>
 </sst>
 </file>
@@ -1289,32 +1282,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L59" sqref="L59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
-    <col min="7" max="8" width="12.5546875" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="7" max="8" width="12.5703125" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5546875" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="14" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" customWidth="1"/>
+    <col min="10" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.28515625" customWidth="1"/>
+    <col min="13" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.2">
+    <row r="1" spans="1:16" ht="61.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.4">
+    <row r="2" spans="1:16" ht="23.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1322,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.2">
+    <row r="3" spans="1:16" ht="61.5">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1341,37 +1334,37 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1153</v>
+        <v>1330</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
         <v>1444</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24.9" customHeight="1">
+    <row r="4" spans="1:16" ht="24.95" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>0.74944237918215617</v>
+        <v>0.73022312373225151</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.2602230483271375</v>
+        <v>1.2279049550854824</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0594795539033457</v>
+        <v>1.0323094755143436</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.85724907063197031</v>
+        <v>0.9634888438133874</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0736059479553903</v>
+        <v>1.0460736018545349</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3763,8 +3756,17 @@
       <c r="G57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" ht="15">
+      <c r="K57" s="3">
+        <v>45909</v>
+      </c>
+      <c r="L57" t="s">
+        <v>212</v>
+      </c>
+      <c r="M57">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16">
       <c r="B58" s="3">
         <v>45906</v>
       </c>
@@ -3782,6 +3784,15 @@
       </c>
       <c r="G58">
         <v>38</v>
+      </c>
+      <c r="K58" s="3">
+        <v>45909</v>
+      </c>
+      <c r="L58" t="s">
+        <v>213</v>
+      </c>
+      <c r="M58">
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="2:16">

</xml_diff>

<commit_message>
feat: poprawa paneli lekarz oraz recepcja home
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek\Documents\GitHub\Projekt-Przychodnia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbist\OneDrive\Dokumenty\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B889A8-1B86-448C-8C0F-617311050B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F2CB12-2C0E-43B0-9247-118B5275E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="221">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -690,6 +690,12 @@
   </si>
   <si>
     <t>login</t>
+  </si>
+  <si>
+    <t>lekarz-home.component.ts</t>
+  </si>
+  <si>
+    <t>recepcja-home.component.ts</t>
   </si>
 </sst>
 </file>
@@ -1310,32 +1316,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="D58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
-    <col min="7" max="8" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="7" max="8" width="12.5546875" customWidth="1"/>
     <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="23.28515625" customWidth="1"/>
-    <col min="13" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" customWidth="1"/>
+    <col min="10" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" customWidth="1"/>
+    <col min="13" max="14" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="61.5">
+    <row r="1" spans="1:16" ht="61.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="23.25">
+    <row r="2" spans="1:16" ht="23.4">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1343,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="61.5">
+    <row r="3" spans="1:16" ht="61.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1362,37 +1368,37 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1348</v>
+        <v>1399</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
         <v>1444</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="24.95" customHeight="1">
+    <row r="4" spans="1:16" ht="24.9" customHeight="1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0209987885314309</v>
+        <v>1.0140374331550801</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1407995692556199</v>
+        <v>1.1330213903743316</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.95907928388746799</v>
+        <v>0.95254010695187163</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.9072553506528469</v>
+        <v>0.93516042780748665</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.97186700767263423</v>
+        <v>0.96524064171122992</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -3794,7 +3800,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" ht="15">
       <c r="B58" s="3">
         <v>45906</v>
       </c>
@@ -3997,7 +4003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:7">
+    <row r="65" spans="2:13">
       <c r="B65" s="3">
         <v>45906</v>
       </c>
@@ -4016,8 +4022,17 @@
       <c r="G65">
         <v>11</v>
       </c>
-    </row>
-    <row r="66" spans="2:7">
+      <c r="K65" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L65" t="s">
+        <v>163</v>
+      </c>
+      <c r="M65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13">
       <c r="B66" s="3">
         <v>45906</v>
       </c>
@@ -4036,8 +4051,17 @@
       <c r="G66">
         <v>16</v>
       </c>
-    </row>
-    <row r="67" spans="2:7">
+      <c r="K66" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L66" t="s">
+        <v>219</v>
+      </c>
+      <c r="M66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13">
       <c r="B67" s="3">
         <v>45906</v>
       </c>
@@ -4056,8 +4080,17 @@
       <c r="G67">
         <v>75</v>
       </c>
-    </row>
-    <row r="68" spans="2:7">
+      <c r="K67" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L67" t="s">
+        <v>191</v>
+      </c>
+      <c r="M67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13">
       <c r="B68" s="3">
         <v>45906</v>
       </c>
@@ -4076,8 +4109,17 @@
       <c r="G68">
         <v>16</v>
       </c>
-    </row>
-    <row r="69" spans="2:7">
+      <c r="K68" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L68" t="s">
+        <v>220</v>
+      </c>
+      <c r="M68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13">
       <c r="B69" s="3">
         <v>45906</v>
       </c>
@@ -4096,8 +4138,17 @@
       <c r="G69">
         <v>20</v>
       </c>
-    </row>
-    <row r="70" spans="2:7">
+      <c r="K69" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L69" t="s">
+        <v>181</v>
+      </c>
+      <c r="M69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13">
       <c r="B70" s="3">
         <v>45906</v>
       </c>
@@ -4116,8 +4167,17 @@
       <c r="G70">
         <v>19</v>
       </c>
-    </row>
-    <row r="71" spans="2:7">
+      <c r="K70" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L70" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="M70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13">
       <c r="B71" s="3">
         <v>45906</v>
       </c>
@@ -4137,7 +4197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="2:7">
+    <row r="72" spans="2:13">
       <c r="B72" s="3">
         <v>45906</v>
       </c>
@@ -4157,7 +4217,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="2:7">
+    <row r="73" spans="2:13">
       <c r="B73" s="3">
         <v>45906</v>
       </c>
@@ -4177,7 +4237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="2:7">
+    <row r="74" spans="2:13">
       <c r="B74" s="3">
         <v>45906</v>
       </c>
@@ -4197,7 +4257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="2:7">
+    <row r="75" spans="2:13">
       <c r="B75" s="3">
         <v>45910</v>
       </c>
@@ -4217,7 +4277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="2:7">
+    <row r="76" spans="2:13">
       <c r="B76" s="3">
         <v>45910</v>
       </c>
@@ -4237,7 +4297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="2:7">
+    <row r="77" spans="2:13">
       <c r="B77" s="3">
         <v>45910</v>
       </c>
@@ -4257,7 +4317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="2:7">
+    <row r="78" spans="2:13">
       <c r="B78" s="3">
         <v>45910</v>
       </c>
@@ -4277,7 +4337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="2:7">
+    <row r="79" spans="2:13">
       <c r="B79" s="3">
         <v>45910</v>
       </c>
@@ -4297,7 +4357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="2:7">
+    <row r="80" spans="2:13">
       <c r="B80" s="3">
         <v>45910</v>
       </c>

</xml_diff>

<commit_message>
feat: css update dla paneli logowanie oraz rejestracja & naprawa harmonogramu
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbist\OneDrive\Dokumenty\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F2CB12-2C0E-43B0-9247-118B5275E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A0863B-EF8D-4AD3-856F-7A9BCD77D849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="221">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -1317,7 +1317,7 @@
   <dimension ref="A1:P112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L71" sqref="L71"/>
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1399</v>
+        <v>1494</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -1382,23 +1382,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0140374331550801</v>
+        <v>1.0013201320132012</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1330213903743316</v>
+        <v>1.1188118811881189</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.95254010695187163</v>
+        <v>0.94059405940594054</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.93516042780748665</v>
+        <v>0.98613861386138613</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.96524064171122992</v>
+        <v>0.95313531353135317</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4196,6 +4196,15 @@
       <c r="G71">
         <v>4</v>
       </c>
+      <c r="K71" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L71" t="s">
+        <v>134</v>
+      </c>
+      <c r="M71">
+        <v>5</v>
+      </c>
     </row>
     <row r="72" spans="2:13">
       <c r="B72" s="3">
@@ -4216,6 +4225,15 @@
       <c r="G72">
         <v>11</v>
       </c>
+      <c r="K72" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L72" t="s">
+        <v>182</v>
+      </c>
+      <c r="M72">
+        <v>35</v>
+      </c>
     </row>
     <row r="73" spans="2:13">
       <c r="B73" s="3">
@@ -4236,6 +4254,15 @@
       <c r="G73">
         <v>6</v>
       </c>
+      <c r="K73" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L73" t="s">
+        <v>183</v>
+      </c>
+      <c r="M73">
+        <v>4</v>
+      </c>
     </row>
     <row r="74" spans="2:13">
       <c r="B74" s="3">
@@ -4256,6 +4283,15 @@
       <c r="G74">
         <v>1</v>
       </c>
+      <c r="K74" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L74" t="s">
+        <v>184</v>
+      </c>
+      <c r="M74">
+        <v>47</v>
+      </c>
     </row>
     <row r="75" spans="2:13">
       <c r="B75" s="3">
@@ -4275,6 +4311,15 @@
       </c>
       <c r="G75">
         <v>1</v>
+      </c>
+      <c r="K75" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L75" t="s">
+        <v>178</v>
+      </c>
+      <c r="M75">
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="2:13">

</xml_diff>

<commit_message>
feat: pacjent-wizyta-add komponent & porzadkowanie komponentow
</commit_message>
<xml_diff>
--- a/Raport.xlsx
+++ b/Raport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pbist\OneDrive\Dokumenty\GitHub\Projekt-Przychodnia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A0863B-EF8D-4AD3-856F-7A9BCD77D849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE2BF74-76BA-49B3-B0BC-AEF3E1CF1946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="224">
   <si>
     <t>Roport zaangażowania</t>
   </si>
@@ -696,6 +696,15 @@
   </si>
   <si>
     <t>recepcja-home.component.ts</t>
+  </si>
+  <si>
+    <t>pacjent-wizyta-add.component.css</t>
+  </si>
+  <si>
+    <t>pacjent-wizyta-add.component.html</t>
+  </si>
+  <si>
+    <t>pacjent-wizyta-add.component.ts</t>
   </si>
 </sst>
 </file>
@@ -1316,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L80" sqref="L80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -1368,7 +1377,7 @@
       </c>
       <c r="M3">
         <f>SUM(M7:M1001)</f>
-        <v>1494</v>
+        <v>1612</v>
       </c>
       <c r="P3">
         <f>SUM(P7:P1001)</f>
@@ -1382,23 +1391,23 @@
       <c r="B4" s="1"/>
       <c r="D4">
         <f>($B$2*D$3)/SUM($D$3:$AK$3)</f>
-        <v>1.0013201320132012</v>
+        <v>0.98596126348628621</v>
       </c>
       <c r="G4">
         <f>($B$2*G$3)/SUM($D$3:$AK$3)</f>
-        <v>1.1188118811881189</v>
+        <v>1.1016508514233718</v>
       </c>
       <c r="J4">
         <f>($B$2*J$3)/SUM($D$3:$AK$3)</f>
-        <v>0.94059405940594054</v>
+        <v>0.92616664500194978</v>
       </c>
       <c r="M4">
         <f>($B$2*M$3)/SUM($D$3:$AK$3)</f>
-        <v>0.98613861386138613</v>
+        <v>1.0477057064864161</v>
       </c>
       <c r="P4">
         <f>($B$2*P$3)/SUM($D$3:$AK$3)</f>
-        <v>0.95313531353135317</v>
+        <v>0.93851553360197582</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4341,6 +4350,15 @@
       <c r="G76">
         <v>2</v>
       </c>
+      <c r="K76" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L76" t="s">
+        <v>221</v>
+      </c>
+      <c r="M76">
+        <v>69</v>
+      </c>
     </row>
     <row r="77" spans="2:13">
       <c r="B77" s="3">
@@ -4361,6 +4379,15 @@
       <c r="G77">
         <v>12</v>
       </c>
+      <c r="K77" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L77" t="s">
+        <v>222</v>
+      </c>
+      <c r="M77">
+        <v>21</v>
+      </c>
     </row>
     <row r="78" spans="2:13">
       <c r="B78" s="3">
@@ -4381,6 +4408,15 @@
       <c r="G78">
         <v>3</v>
       </c>
+      <c r="K78" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L78" t="s">
+        <v>223</v>
+      </c>
+      <c r="M78">
+        <v>26</v>
+      </c>
     </row>
     <row r="79" spans="2:13">
       <c r="B79" s="3">
@@ -4401,6 +4437,15 @@
       <c r="G79">
         <v>30</v>
       </c>
+      <c r="K79" s="3">
+        <v>45911</v>
+      </c>
+      <c r="L79" t="s">
+        <v>130</v>
+      </c>
+      <c r="M79">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="2:13">
       <c r="B80" s="3">
@@ -4421,8 +4466,9 @@
       <c r="G80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="2:7">
+      <c r="K80" s="3"/>
+    </row>
+    <row r="81" spans="2:11">
       <c r="B81" s="3">
         <v>45910</v>
       </c>
@@ -4441,8 +4487,9 @@
       <c r="G81">
         <v>6</v>
       </c>
-    </row>
-    <row r="82" spans="2:7">
+      <c r="K81" s="3"/>
+    </row>
+    <row r="82" spans="2:11">
       <c r="B82" s="3">
         <v>45910</v>
       </c>
@@ -4462,7 +4509,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:11">
       <c r="B83" s="3">
         <v>45910</v>
       </c>
@@ -4482,7 +4529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:11">
       <c r="B84" s="3">
         <v>45910</v>
       </c>
@@ -4502,7 +4549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:11">
       <c r="B85" s="3">
         <v>45910</v>
       </c>
@@ -4522,7 +4569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:11">
       <c r="B86" s="3">
         <v>45910</v>
       </c>
@@ -4542,7 +4589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:11">
       <c r="B87" s="3">
         <v>45910</v>
       </c>
@@ -4562,7 +4609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="2:7">
+    <row r="88" spans="2:11">
       <c r="B88" s="3">
         <v>45910</v>
       </c>
@@ -4582,7 +4629,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="2:7">
+    <row r="89" spans="2:11">
       <c r="E89" s="3">
         <v>45883</v>
       </c>
@@ -4593,7 +4640,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="90" spans="2:7">
+    <row r="90" spans="2:11">
       <c r="E90" s="3">
         <v>45883</v>
       </c>
@@ -4604,7 +4651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:7">
+    <row r="91" spans="2:11">
       <c r="E91" s="3">
         <v>45883</v>
       </c>
@@ -4615,7 +4662,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="92" spans="2:7">
+    <row r="92" spans="2:11">
       <c r="E92" s="3">
         <v>45883</v>
       </c>
@@ -4626,7 +4673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:7">
+    <row r="93" spans="2:11">
       <c r="E93" s="3">
         <v>45883</v>
       </c>
@@ -4637,7 +4684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="2:7">
+    <row r="94" spans="2:11">
       <c r="E94" s="3">
         <v>45883</v>
       </c>
@@ -4648,7 +4695,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="2:7">
+    <row r="95" spans="2:11">
       <c r="E95" s="3">
         <v>45895</v>
       </c>
@@ -4659,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="2:7">
+    <row r="96" spans="2:11">
       <c r="E96" s="3">
         <v>45895</v>
       </c>

</xml_diff>